<commit_message>
Run with less features
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -112,13 +112,36 @@
   <si>
     <t>Change in how NA values are filled (useing mean for fare instead of median and using most common value of Embarked instead of unknown)</t>
   </si>
+  <si>
+    <t>{'criterion': 'gini', 'max_depth': 30, 'max_features': 'auto', 'min_samples_leaf': 3, 'min_samples_split': 3, 'n_estimators': 10}</t>
+  </si>
+  <si>
+    <t>These are all overfitting the data</t>
+  </si>
+  <si>
+    <t>With only top features (using dummy features)</t>
+  </si>
+  <si>
+    <t>With only top 23 features (using dummy features)</t>
+  </si>
+  <si>
+    <t>With only top 31 features (using dummy features)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,6 +164,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,113 +190,149 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -314,6 +381,21 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -362,6 +444,21 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -637,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S213"/>
+  <dimension ref="A1:S217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,7 +748,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -673,23 +770,23 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="2"/>
@@ -975,11 +1072,19 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="1">
+        <v>84.969999999999899</v>
+      </c>
+      <c r="D13" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E13" s="1">
+        <v>83.503121098626707</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
@@ -996,9 +1101,7 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1018,25 +1121,15 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1051,18 +1144,24 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1">
-        <v>91.579999999999899</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <v>77.989999999999995</v>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="1"/>
@@ -1078,24 +1177,18 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1">
-        <v>89.189999999999898</v>
-      </c>
-      <c r="D17" s="1">
-        <v>92.31</v>
-      </c>
-      <c r="E17" s="1">
-        <v>83.732833957552998</v>
-      </c>
+        <v>91.579999999999899</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1">
-        <v>77.033000000000001</v>
+        <v>77.989999999999995</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="1"/>
@@ -1116,15 +1209,19 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
+        <v>89.189999999999898</v>
+      </c>
+      <c r="D18" s="1">
+        <v>92.31</v>
+      </c>
       <c r="E18" s="1">
-        <v>82.835205992509302</v>
+        <v>83.732833957552998</v>
       </c>
       <c r="F18" s="1">
-        <v>75.597999999999999</v>
+        <v>77.033000000000001</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="1"/>
@@ -1140,21 +1237,21 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1">
-        <v>90.73</v>
-      </c>
-      <c r="D19" s="1">
-        <v>82.12</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1">
-        <v>81.932584269662897</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>82.835205992509302</v>
+      </c>
+      <c r="F19" s="1">
+        <v>75.597999999999999</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1169,26 +1266,24 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="1">
-        <v>85.39</v>
+        <v>90.73</v>
       </c>
       <c r="D20" s="1">
         <v>82.12</v>
       </c>
       <c r="E20" s="1">
-        <v>83.169787765293293</v>
-      </c>
-      <c r="F20" s="1">
-        <v>77.989999999999995</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>81.932584269662897</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1202,22 +1297,24 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C21" s="1">
-        <v>90.73</v>
+        <v>85.39</v>
       </c>
       <c r="D21" s="1">
-        <v>82.68</v>
+        <v>82.12</v>
       </c>
       <c r="E21" s="1">
         <v>83.169787765293293</v>
       </c>
       <c r="F21" s="1">
-        <v>76.075999999999993</v>
+        <v>77.989999999999995</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="1"/>
@@ -1233,24 +1330,22 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="C22" s="1">
-        <v>85.39</v>
+        <v>90.73</v>
       </c>
       <c r="D22" s="1">
-        <v>81.56</v>
+        <v>82.68</v>
       </c>
       <c r="E22" s="1">
         <v>83.169787765293293</v>
       </c>
       <c r="F22" s="1">
-        <v>77.510999999999996</v>
+        <v>76.075999999999993</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="1"/>
@@ -1266,24 +1361,26 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C23" s="1">
-        <v>91.01</v>
+        <v>85.39</v>
       </c>
       <c r="D23" s="1">
-        <v>81.010000000000005</v>
+        <v>81.56</v>
       </c>
       <c r="E23" s="1">
-        <v>81.821473158551797</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>83.169787765293293</v>
+      </c>
+      <c r="F23" s="1">
+        <v>77.510999999999996</v>
+      </c>
+      <c r="G23" s="2"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1298,13 +1395,23 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="C24" s="1">
+        <v>91.01</v>
+      </c>
+      <c r="D24" s="1">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="E24" s="1">
+        <v>81.821473158551797</v>
+      </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1318,15 +1425,25 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1">
+        <v>85.25</v>
+      </c>
+      <c r="D25" s="1">
+        <v>79.89</v>
+      </c>
+      <c r="E25" s="1">
+        <v>82.389513108614196</v>
+      </c>
+      <c r="F25">
+        <v>77.033000000000001</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1341,25 +1458,14 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="G26" s="2"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1374,20 +1480,12 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1">
-        <v>90.73</v>
-      </c>
-      <c r="D27" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E27" s="1">
-        <v>81.932584269662897</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="1"/>
@@ -1403,25 +1501,15 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="1">
-        <v>85.39</v>
-      </c>
-      <c r="D28" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E28" s="1">
-        <v>83.169787765293293</v>
-      </c>
-      <c r="F28" s="1">
-        <v>77.989999999999995</v>
-      </c>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="2"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1437,12 +1525,24 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="A29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1457,14 +1557,20 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="C30" s="1">
+        <v>90.73</v>
+      </c>
+      <c r="D30" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E30" s="1">
+        <v>81.932584269662897</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
       <c r="H30" s="1"/>
@@ -1480,24 +1586,24 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C31" s="1">
+        <v>85.39</v>
+      </c>
+      <c r="D31" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E31" s="1">
+        <v>83.169787765293293</v>
+      </c>
+      <c r="F31" s="1">
+        <v>77.989999999999995</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="1"/>
@@ -1514,22 +1620,12 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1">
-        <v>86.519999999999897</v>
-      </c>
-      <c r="D32" s="1">
-        <v>80.45</v>
-      </c>
-      <c r="E32" s="1">
-        <v>82.828963795255902</v>
-      </c>
-      <c r="F32" s="1">
-        <v>77.510999999999996</v>
-      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="2"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1544,23 +1640,13 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1">
-        <v>86.379999999999896</v>
-      </c>
-      <c r="D33" s="1">
-        <v>81.010000000000005</v>
-      </c>
-      <c r="E33" s="1">
-        <v>82.942571785268399</v>
-      </c>
-      <c r="F33" s="1">
-        <v>75.597999999999999</v>
-      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="G33" s="2"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1575,25 +1661,15 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="1">
-        <v>85.81</v>
-      </c>
-      <c r="D34" s="1">
-        <v>79.329999999999899</v>
-      </c>
-      <c r="E34" s="1">
-        <v>82.831460674157299</v>
-      </c>
-      <c r="F34" s="1">
-        <v>77.510999999999996</v>
-      </c>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="2"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1608,24 +1684,24 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="1">
-        <v>84.829999999999899</v>
-      </c>
-      <c r="D35" s="1">
-        <v>79.89</v>
-      </c>
-      <c r="E35" s="1">
-        <v>82.8252184769038</v>
-      </c>
-      <c r="F35" s="1">
-        <v>77.510999999999996</v>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="1"/>
@@ -1642,12 +1718,22 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="C36" s="1">
+        <v>86.519999999999897</v>
+      </c>
+      <c r="D36" s="1">
+        <v>80.45</v>
+      </c>
+      <c r="E36" s="1">
+        <v>82.828963795255902</v>
+      </c>
+      <c r="F36" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1662,13 +1748,23 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
+    <row r="37" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="C37" s="1">
+        <v>86.379999999999896</v>
+      </c>
+      <c r="D37" s="1">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="E37" s="1">
+        <v>82.942571785268399</v>
+      </c>
+      <c r="F37" s="1">
+        <v>75.597999999999999</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -1683,13 +1779,25 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+    <row r="38" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="1">
+        <v>85.81</v>
+      </c>
+      <c r="D38" s="1">
+        <v>79.329999999999899</v>
+      </c>
+      <c r="E38" s="1">
+        <v>82.831460674157299</v>
+      </c>
+      <c r="F38" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -1704,13 +1812,25 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+    <row r="39" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="1">
+        <v>84.829999999999899</v>
+      </c>
+      <c r="D39" s="1">
+        <v>79.89</v>
+      </c>
+      <c r="E39" s="1">
+        <v>82.8252184769038</v>
+      </c>
+      <c r="F39" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -4168,7 +4288,7 @@
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
-      <c r="G156" s="1"/>
+      <c r="G156" s="2"/>
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
       <c r="J156" s="1"/>
@@ -4189,7 +4309,7 @@
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
+      <c r="G157" s="2"/>
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="1"/>
@@ -4210,7 +4330,7 @@
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
+      <c r="G158" s="2"/>
       <c r="H158" s="1"/>
       <c r="I158" s="1"/>
       <c r="J158" s="1"/>
@@ -4231,7 +4351,7 @@
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
+      <c r="G159" s="2"/>
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
       <c r="J159" s="1"/>
@@ -5379,6 +5499,90 @@
       <c r="R213" s="1"/>
       <c r="S213" s="1"/>
     </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
+      <c r="C214" s="1"/>
+      <c r="D214" s="1"/>
+      <c r="E214" s="1"/>
+      <c r="F214" s="1"/>
+      <c r="G214" s="1"/>
+      <c r="H214" s="1"/>
+      <c r="I214" s="1"/>
+      <c r="J214" s="1"/>
+      <c r="K214" s="1"/>
+      <c r="L214" s="1"/>
+      <c r="M214" s="1"/>
+      <c r="N214" s="1"/>
+      <c r="O214" s="1"/>
+      <c r="P214" s="1"/>
+      <c r="Q214" s="1"/>
+      <c r="R214" s="1"/>
+      <c r="S214" s="1"/>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A215" s="1"/>
+      <c r="B215" s="1"/>
+      <c r="C215" s="1"/>
+      <c r="D215" s="1"/>
+      <c r="E215" s="1"/>
+      <c r="F215" s="1"/>
+      <c r="G215" s="1"/>
+      <c r="H215" s="1"/>
+      <c r="I215" s="1"/>
+      <c r="J215" s="1"/>
+      <c r="K215" s="1"/>
+      <c r="L215" s="1"/>
+      <c r="M215" s="1"/>
+      <c r="N215" s="1"/>
+      <c r="O215" s="1"/>
+      <c r="P215" s="1"/>
+      <c r="Q215" s="1"/>
+      <c r="R215" s="1"/>
+      <c r="S215" s="1"/>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="E216" s="1"/>
+      <c r="F216" s="1"/>
+      <c r="G216" s="1"/>
+      <c r="H216" s="1"/>
+      <c r="I216" s="1"/>
+      <c r="J216" s="1"/>
+      <c r="K216" s="1"/>
+      <c r="L216" s="1"/>
+      <c r="M216" s="1"/>
+      <c r="N216" s="1"/>
+      <c r="O216" s="1"/>
+      <c r="P216" s="1"/>
+      <c r="Q216" s="1"/>
+      <c r="R216" s="1"/>
+      <c r="S216" s="1"/>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="1"/>
+      <c r="H217" s="1"/>
+      <c r="I217" s="1"/>
+      <c r="J217" s="1"/>
+      <c r="K217" s="1"/>
+      <c r="L217" s="1"/>
+      <c r="M217" s="1"/>
+      <c r="N217" s="1"/>
+      <c r="O217" s="1"/>
+      <c r="P217" s="1"/>
+      <c r="Q217" s="1"/>
+      <c r="R217" s="1"/>
+      <c r="S217" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Run with even less features
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -127,6 +127,12 @@
   <si>
     <t>With only top 31 features (using dummy features)</t>
   </si>
+  <si>
+    <t>{n_estimators=10}</t>
+  </si>
+  <si>
+    <t>Title_Mr, "Sex", "Title_Mrs", "Pclass_3", "Title_Miss", "Cabin_NA", "Fare_0", "Age_3", "Age_2", "Embarked_C"</t>
+  </si>
 </sst>
 </file>
 
@@ -190,8 +196,74 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -332,7 +404,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -396,6 +468,39 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -459,6 +564,39 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S217"/>
+  <dimension ref="A1:S218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1480,13 +1618,14 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1502,9 +1641,7 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1525,24 +1662,14 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="2"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1557,21 +1684,25 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1">
-        <v>90.73</v>
-      </c>
-      <c r="D30" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E30" s="1">
-        <v>81.932584269662897</v>
-      </c>
-      <c r="F30" s="1"/>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1586,25 +1717,21 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B31" s="1"/>
       <c r="C31" s="1">
-        <v>85.39</v>
+        <v>90.73</v>
       </c>
       <c r="D31" s="1">
         <v>82.12</v>
       </c>
       <c r="E31" s="1">
-        <v>83.169787765293293</v>
-      </c>
-      <c r="F31" s="1">
-        <v>77.989999999999995</v>
-      </c>
+        <v>81.932584269662897</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="2"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1619,13 +1746,25 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+    <row r="32" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1">
+        <v>85.39</v>
+      </c>
+      <c r="D32" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E32" s="1">
+        <v>83.169787765293293</v>
+      </c>
+      <c r="F32" s="1">
+        <v>77.989999999999995</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1662,9 +1801,7 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1685,24 +1822,14 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="2"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1718,21 +1845,23 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1">
-        <v>86.519999999999897</v>
-      </c>
-      <c r="D36" s="1">
-        <v>80.45</v>
-      </c>
-      <c r="E36" s="1">
-        <v>82.828963795255902</v>
-      </c>
-      <c r="F36" s="1">
-        <v>77.510999999999996</v>
+      <c r="A36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="1"/>
@@ -1748,22 +1877,22 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
-        <v>86.379999999999896</v>
+        <v>86.519999999999897</v>
       </c>
       <c r="D37" s="1">
-        <v>81.010000000000005</v>
+        <v>80.45</v>
       </c>
       <c r="E37" s="1">
-        <v>82.942571785268399</v>
+        <v>82.828963795255902</v>
       </c>
       <c r="F37" s="1">
-        <v>75.597999999999999</v>
+        <v>77.510999999999996</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="1"/>
@@ -1779,24 +1908,22 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B38" s="1"/>
       <c r="C38" s="1">
-        <v>85.81</v>
+        <v>86.379999999999896</v>
       </c>
       <c r="D38" s="1">
-        <v>79.329999999999899</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="E38" s="1">
-        <v>82.831460674157299</v>
+        <v>82.942571785268399</v>
       </c>
       <c r="F38" s="1">
-        <v>77.510999999999996</v>
+        <v>75.597999999999999</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="1"/>
@@ -1814,19 +1941,19 @@
     </row>
     <row r="39" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="1">
-        <v>84.829999999999899</v>
+        <v>85.81</v>
       </c>
       <c r="D39" s="1">
-        <v>79.89</v>
+        <v>79.329999999999899</v>
       </c>
       <c r="E39" s="1">
-        <v>82.8252184769038</v>
+        <v>82.831460674157299</v>
       </c>
       <c r="F39" s="1">
         <v>77.510999999999996</v>
@@ -1845,13 +1972,25 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+    <row r="40" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1">
+        <v>84.829999999999899</v>
+      </c>
+      <c r="D40" s="1">
+        <v>79.89</v>
+      </c>
+      <c r="E40" s="1">
+        <v>82.8252184769038</v>
+      </c>
+      <c r="F40" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -4372,7 +4511,7 @@
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
-      <c r="G160" s="1"/>
+      <c r="G160" s="2"/>
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
       <c r="J160" s="1"/>
@@ -5583,6 +5722,27 @@
       <c r="R217" s="1"/>
       <c r="S217" s="1"/>
     </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A218" s="1"/>
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1"/>
+      <c r="E218" s="1"/>
+      <c r="F218" s="1"/>
+      <c r="G218" s="1"/>
+      <c r="H218" s="1"/>
+      <c r="I218" s="1"/>
+      <c r="J218" s="1"/>
+      <c r="K218" s="1"/>
+      <c r="L218" s="1"/>
+      <c r="M218" s="1"/>
+      <c r="N218" s="1"/>
+      <c r="O218" s="1"/>
+      <c r="P218" s="1"/>
+      <c r="Q218" s="1"/>
+      <c r="R218" s="1"/>
+      <c r="S218" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updates to notes and readme
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="480" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="920" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -133,6 +133,9 @@
   <si>
     <t>Title_Mr, "Sex", "Title_Mrs", "Pclass_3", "Title_Miss", "Cabin_NA", "Fare_0", "Age_3", "Age_2", "Embarked_C"</t>
   </si>
+  <si>
+    <t>{'criterion': 'entropy', 'max_depth': 100, 'max_features': 'auto', 'min_samples_leaf': 1, 'min_samples_split': 10, 'n_estimators': 10}</t>
+  </si>
 </sst>
 </file>
 
@@ -196,8 +199,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="193">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,7 +437,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="193">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -501,6 +534,21 @@
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -597,6 +645,21 @@
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -874,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -1618,14 +1681,25 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="1">
+        <v>83.989999999999895</v>
+      </c>
+      <c r="D27" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E27" s="1">
+        <v>81.029962546816407</v>
+      </c>
+      <c r="F27">
+        <v>78.947000000000003</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>

</xml_diff>

<commit_message>
Trying with different number of features
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -136,6 +136,30 @@
   <si>
     <t>{'criterion': 'entropy', 'max_depth': 100, 'max_features': 'auto', 'min_samples_leaf': 1, 'min_samples_split': 10, 'n_estimators': 10}</t>
   </si>
+  <si>
+    <t>Title_Mr, "Sex", "Title_Mrs", "Pclass_3", "Title_Miss", "Cabin_NA", "Fare_0"</t>
+  </si>
+  <si>
+    <t>Used less features to stop overfitting</t>
+  </si>
+  <si>
+    <t>{'criterion': 'entropy', 'max_depth': 30, 'max_features': 'sqrt', 'min_samples_leaf': 10, 'min_samples_split': 10, 'n_estimators': 10}</t>
+  </si>
+  <si>
+    <t>Title_Mr, "Sex", "Title_Mrs", "Pclass_3", "Title_Miss"</t>
+  </si>
+  <si>
+    <t>{'criterion': 'gini', 'max_depth': 3, 'max_features': 'sqrt', 'min_samples_leaf': 10, 'min_samples_split': 30, 'n_estimators': 10}</t>
+  </si>
+  <si>
+    <t>Not going to test this model</t>
+  </si>
+  <si>
+    <t>Title_Mr, "Sex", "Title_Mrs", "Pclass_3", "Title_Miss", "Cabin_NA", "Fare_0", "Age_3", "Age_2", "Embarked_C", "Age_4", "LargeFamily", "Pclass_1", "Pclass_2", "Embarked_S"</t>
+  </si>
+  <si>
+    <t>{'criterion': 'entropy', 'max_depth': 100, 'max_features': 'sqrt', 'min_samples_leaf': 3, 'min_samples_split': 3, 'n_estimators': 100}</t>
+  </si>
 </sst>
 </file>
 
@@ -199,8 +223,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="223">
+  <cellStyleXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -437,7 +485,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="223">
+  <cellStyles count="247">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -549,6 +597,18 @@
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -660,6 +720,18 @@
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -935,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S218"/>
+  <dimension ref="A1:S221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1700,7 +1772,9 @@
       <c r="F27">
         <v>78.947000000000003</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1714,13 +1788,25 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+    <row r="28" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1">
+        <v>82.019999999999897</v>
+      </c>
+      <c r="D28" s="1">
+        <v>80.45</v>
+      </c>
+      <c r="E28" s="1">
+        <v>80.360799001248395</v>
+      </c>
+      <c r="F28">
+        <v>78.947000000000003</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1735,16 +1821,25 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="2"/>
+    <row r="29" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1">
+        <v>79.069999999999894</v>
+      </c>
+      <c r="D29" s="1">
+        <v>78.209999999999894</v>
+      </c>
+      <c r="E29" s="1">
+        <v>78.1111111111111</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1758,24 +1853,24 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>5</v>
+    <row r="30" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="1">
+        <v>84.829999999999899</v>
+      </c>
+      <c r="D30" s="1">
+        <v>83.799999999999898</v>
+      </c>
+      <c r="E30" s="1">
+        <v>83.277153558052404</v>
+      </c>
+      <c r="F30">
+        <v>77.510999999999996</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="1"/>
@@ -1791,20 +1886,12 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1">
-        <v>90.73</v>
-      </c>
-      <c r="D31" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E31" s="1">
-        <v>81.932584269662897</v>
-      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="2"/>
       <c r="H31" s="1"/>
@@ -1820,25 +1907,15 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="1">
-        <v>85.39</v>
-      </c>
-      <c r="D32" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E32" s="1">
-        <v>83.169787765293293</v>
-      </c>
-      <c r="F32" s="1">
-        <v>77.989999999999995</v>
-      </c>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="2"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1854,12 +1931,24 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1874,12 +1963,20 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
+    <row r="34" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="C34" s="1">
+        <v>90.73</v>
+      </c>
+      <c r="D34" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E34" s="1">
+        <v>81.932584269662897</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="2"/>
       <c r="H34" s="1"/>
@@ -1895,15 +1992,25 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+    <row r="35" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1">
+        <v>85.39</v>
+      </c>
+      <c r="D35" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E35" s="1">
+        <v>83.169787765293293</v>
+      </c>
+      <c r="F35" s="1">
+        <v>77.989999999999995</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1919,24 +2026,12 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1952,22 +2047,12 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="1">
-        <v>86.519999999999897</v>
-      </c>
-      <c r="D37" s="1">
-        <v>80.45</v>
-      </c>
-      <c r="E37" s="1">
-        <v>82.828963795255902</v>
-      </c>
-      <c r="F37" s="1">
-        <v>77.510999999999996</v>
-      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="G37" s="2"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -1982,23 +2067,15 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>15</v>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B38" s="1"/>
-      <c r="C38" s="1">
-        <v>86.379999999999896</v>
-      </c>
-      <c r="D38" s="1">
-        <v>81.010000000000005</v>
-      </c>
-      <c r="E38" s="1">
-        <v>82.942571785268399</v>
-      </c>
-      <c r="F38" s="1">
-        <v>75.597999999999999</v>
-      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="G38" s="2"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2013,24 +2090,24 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="1">
-        <v>85.81</v>
-      </c>
-      <c r="D39" s="1">
-        <v>79.329999999999899</v>
-      </c>
-      <c r="E39" s="1">
-        <v>82.831460674157299</v>
-      </c>
-      <c r="F39" s="1">
-        <v>77.510999999999996</v>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="1"/>
@@ -2046,21 +2123,19 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B40" s="1"/>
       <c r="C40" s="1">
-        <v>84.829999999999899</v>
+        <v>86.519999999999897</v>
       </c>
       <c r="D40" s="1">
-        <v>79.89</v>
+        <v>80.45</v>
       </c>
       <c r="E40" s="1">
-        <v>82.8252184769038</v>
+        <v>82.828963795255902</v>
       </c>
       <c r="F40" s="1">
         <v>77.510999999999996</v>
@@ -2079,13 +2154,23 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
+    <row r="41" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="C41" s="1">
+        <v>86.379999999999896</v>
+      </c>
+      <c r="D41" s="1">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="E41" s="1">
+        <v>82.942571785268399</v>
+      </c>
+      <c r="F41" s="1">
+        <v>75.597999999999999</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2100,13 +2185,25 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+    <row r="42" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="1">
+        <v>85.81</v>
+      </c>
+      <c r="D42" s="1">
+        <v>79.329999999999899</v>
+      </c>
+      <c r="E42" s="1">
+        <v>82.831460674157299</v>
+      </c>
+      <c r="F42" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2121,13 +2218,25 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+    <row r="43" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="1">
+        <v>84.829999999999899</v>
+      </c>
+      <c r="D43" s="1">
+        <v>79.89</v>
+      </c>
+      <c r="E43" s="1">
+        <v>82.8252184769038</v>
+      </c>
+      <c r="F43" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -4606,7 +4715,7 @@
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
-      <c r="G161" s="1"/>
+      <c r="G161" s="2"/>
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
       <c r="J161" s="1"/>
@@ -4627,7 +4736,7 @@
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
-      <c r="G162" s="1"/>
+      <c r="G162" s="2"/>
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
       <c r="J162" s="1"/>
@@ -4648,7 +4757,7 @@
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
-      <c r="G163" s="1"/>
+      <c r="G163" s="2"/>
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
       <c r="J163" s="1"/>
@@ -5817,6 +5926,69 @@
       <c r="R218" s="1"/>
       <c r="S218" s="1"/>
     </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1"/>
+      <c r="E219" s="1"/>
+      <c r="F219" s="1"/>
+      <c r="G219" s="1"/>
+      <c r="H219" s="1"/>
+      <c r="I219" s="1"/>
+      <c r="J219" s="1"/>
+      <c r="K219" s="1"/>
+      <c r="L219" s="1"/>
+      <c r="M219" s="1"/>
+      <c r="N219" s="1"/>
+      <c r="O219" s="1"/>
+      <c r="P219" s="1"/>
+      <c r="Q219" s="1"/>
+      <c r="R219" s="1"/>
+      <c r="S219" s="1"/>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="1"/>
+      <c r="G220" s="1"/>
+      <c r="H220" s="1"/>
+      <c r="I220" s="1"/>
+      <c r="J220" s="1"/>
+      <c r="K220" s="1"/>
+      <c r="L220" s="1"/>
+      <c r="M220" s="1"/>
+      <c r="N220" s="1"/>
+      <c r="O220" s="1"/>
+      <c r="P220" s="1"/>
+      <c r="Q220" s="1"/>
+      <c r="R220" s="1"/>
+      <c r="S220" s="1"/>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="1"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="1"/>
+      <c r="G221" s="1"/>
+      <c r="H221" s="1"/>
+      <c r="I221" s="1"/>
+      <c r="J221" s="1"/>
+      <c r="K221" s="1"/>
+      <c r="L221" s="1"/>
+      <c r="M221" s="1"/>
+      <c r="N221" s="1"/>
+      <c r="O221" s="1"/>
+      <c r="P221" s="1"/>
+      <c r="Q221" s="1"/>
+      <c r="R221" s="1"/>
+      <c r="S221" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
10 features is working best
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -160,6 +160,15 @@
   <si>
     <t>{'criterion': 'entropy', 'max_depth': 100, 'max_features': 'sqrt', 'min_samples_leaf': 3, 'min_samples_split': 3, 'n_estimators': 100}</t>
   </si>
+  <si>
+    <t>Title_Mr, "Sex", "Title_Mrs", "Pclass_3", "Title_Miss", "Cabin_NA", "Fare_0", "Age_3", "Age_2", "Embarked_C", "Age_4", "LargeFamily", "Pclass_1"</t>
+  </si>
+  <si>
+    <t>{'criterion': 'entropy', 'max_depth': 100, 'max_features': 'auto', 'min_samples_leaf': 1, 'min_samples_split': 10, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>I don't think the grid search I am doing it very good</t>
+  </si>
 </sst>
 </file>
 
@@ -223,8 +232,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="247">
+  <cellStyleXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,7 +518,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="247">
+  <cellStyles count="271">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -609,6 +642,18 @@
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -732,6 +777,18 @@
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1007,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S221"/>
+  <dimension ref="A1:S223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1886,13 +1943,25 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+    <row r="31" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1">
+        <v>85.53</v>
+      </c>
+      <c r="D31" s="1">
+        <v>82.68</v>
+      </c>
+      <c r="E31" s="1">
+        <v>82.157303370786494</v>
+      </c>
+      <c r="F31">
+        <v>77.033000000000001</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1907,16 +1976,26 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>19</v>
+    <row r="32" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="2"/>
+      <c r="C32" s="1">
+        <v>84.129999999999896</v>
+      </c>
+      <c r="D32" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E32" s="1">
+        <v>81.031210986267098</v>
+      </c>
+      <c r="F32">
+        <v>79.903999999999996</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1931,24 +2010,12 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="G33" s="2"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1963,20 +2030,14 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>15</v>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="1">
-        <v>90.73</v>
-      </c>
-      <c r="D34" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E34" s="1">
-        <v>81.932584269662897</v>
-      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="2"/>
       <c r="H34" s="1"/>
@@ -1992,24 +2053,24 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="1">
-        <v>85.39</v>
-      </c>
-      <c r="D35" s="1">
-        <v>82.12</v>
-      </c>
-      <c r="E35" s="1">
-        <v>83.169787765293293</v>
-      </c>
-      <c r="F35" s="1">
-        <v>77.989999999999995</v>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="1"/>
@@ -2025,12 +2086,20 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
+    <row r="36" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="C36" s="1">
+        <v>90.73</v>
+      </c>
+      <c r="D36" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E36" s="1">
+        <v>81.932584269662897</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="2"/>
       <c r="H36" s="1"/>
@@ -2046,13 +2115,25 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+    <row r="37" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="1">
+        <v>85.39</v>
+      </c>
+      <c r="D37" s="1">
+        <v>82.12</v>
+      </c>
+      <c r="E37" s="1">
+        <v>83.169787765293293</v>
+      </c>
+      <c r="F37" s="1">
+        <v>77.989999999999995</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -2068,9 +2149,7 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2091,24 +2170,12 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
       <c r="G39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2124,22 +2191,14 @@
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>22</v>
+      <c r="A40" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B40" s="1"/>
-      <c r="C40" s="1">
-        <v>86.519999999999897</v>
-      </c>
-      <c r="D40" s="1">
-        <v>80.45</v>
-      </c>
-      <c r="E40" s="1">
-        <v>82.828963795255902</v>
-      </c>
-      <c r="F40" s="1">
-        <v>77.510999999999996</v>
-      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
       <c r="G40" s="2"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2154,22 +2213,24 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1">
-        <v>86.379999999999896</v>
-      </c>
-      <c r="D41" s="1">
-        <v>81.010000000000005</v>
-      </c>
-      <c r="E41" s="1">
-        <v>82.942571785268399</v>
-      </c>
-      <c r="F41" s="1">
-        <v>75.597999999999999</v>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="1"/>
@@ -2185,21 +2246,19 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B42" s="1"/>
       <c r="C42" s="1">
-        <v>85.81</v>
+        <v>86.519999999999897</v>
       </c>
       <c r="D42" s="1">
-        <v>79.329999999999899</v>
+        <v>80.45</v>
       </c>
       <c r="E42" s="1">
-        <v>82.831460674157299</v>
+        <v>82.828963795255902</v>
       </c>
       <c r="F42" s="1">
         <v>77.510999999999996</v>
@@ -2218,24 +2277,22 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B43" s="1"/>
       <c r="C43" s="1">
-        <v>84.829999999999899</v>
+        <v>86.379999999999896</v>
       </c>
       <c r="D43" s="1">
-        <v>79.89</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="E43" s="1">
-        <v>82.8252184769038</v>
+        <v>82.942571785268399</v>
       </c>
       <c r="F43" s="1">
-        <v>77.510999999999996</v>
+        <v>75.597999999999999</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="1"/>
@@ -2251,13 +2308,25 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+    <row r="44" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="1">
+        <v>85.81</v>
+      </c>
+      <c r="D44" s="1">
+        <v>79.329999999999899</v>
+      </c>
+      <c r="E44" s="1">
+        <v>82.831460674157299</v>
+      </c>
+      <c r="F44" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2272,13 +2341,25 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+    <row r="45" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="1">
+        <v>84.829999999999899</v>
+      </c>
+      <c r="D45" s="1">
+        <v>79.89</v>
+      </c>
+      <c r="E45" s="1">
+        <v>82.8252184769038</v>
+      </c>
+      <c r="F45" s="1">
+        <v>77.510999999999996</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -4778,7 +4859,7 @@
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
-      <c r="G164" s="1"/>
+      <c r="G164" s="2"/>
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
       <c r="J164" s="1"/>
@@ -4799,7 +4880,7 @@
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
-      <c r="G165" s="1"/>
+      <c r="G165" s="2"/>
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
       <c r="J165" s="1"/>
@@ -5989,6 +6070,48 @@
       <c r="R221" s="1"/>
       <c r="S221" s="1"/>
     </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
+      <c r="D222" s="1"/>
+      <c r="E222" s="1"/>
+      <c r="F222" s="1"/>
+      <c r="G222" s="1"/>
+      <c r="H222" s="1"/>
+      <c r="I222" s="1"/>
+      <c r="J222" s="1"/>
+      <c r="K222" s="1"/>
+      <c r="L222" s="1"/>
+      <c r="M222" s="1"/>
+      <c r="N222" s="1"/>
+      <c r="O222" s="1"/>
+      <c r="P222" s="1"/>
+      <c r="Q222" s="1"/>
+      <c r="R222" s="1"/>
+      <c r="S222" s="1"/>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="1"/>
+      <c r="G223" s="1"/>
+      <c r="H223" s="1"/>
+      <c r="I223" s="1"/>
+      <c r="J223" s="1"/>
+      <c r="K223" s="1"/>
+      <c r="L223" s="1"/>
+      <c r="M223" s="1"/>
+      <c r="N223" s="1"/>
+      <c r="O223" s="1"/>
+      <c r="P223" s="1"/>
+      <c r="Q223" s="1"/>
+      <c r="R223" s="1"/>
+      <c r="S223" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>